<commit_message>
Added links to pinion, dogbones and battery
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -147,6 +147,9 @@
     <t xml:space="preserve">Dog bone</t>
   </si>
   <si>
+    <t>https://www.amazon.de/-/en/dp/B08FMJXFCH?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -156,7 +159,13 @@
     <t>Pinion</t>
   </si>
   <si>
+    <t>https://www.absima.shop/pp/alu-pinion-32dp/module0-8-20T.htm?shop=absima_en&amp;SessionId=&amp;a=article&amp;ProdNr=2310348&amp;t=19114&amp;c=19132&amp;p=19132</t>
+  </si>
+  <si>
     <t>Battery</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/dp/B08X4GF9DK?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
   </si>
   <si>
     <t>Servo</t>
@@ -261,12 +270,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -794,10 +801,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -811,7 +818,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
@@ -820,54 +827,54 @@
       <c r="D2">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>8</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
@@ -876,20 +883,20 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>8</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="14.25">
       <c r="C8" t="s">
@@ -903,16 +910,16 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3">
-        <v>4</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -920,7 +927,7 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
@@ -929,7 +936,7 @@
       <c r="D10">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -937,7 +944,7 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
@@ -962,10 +969,10 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>2</v>
       </c>
     </row>
@@ -976,10 +983,10 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1004,7 +1011,7 @@
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D17">
@@ -1072,7 +1079,7 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
@@ -1081,15 +1088,15 @@
       <c r="D24">
         <v>4</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1100,10 +1107,13 @@
       <c r="D26">
         <v>4</v>
       </c>
+      <c r="E26" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" ht="14.25">
       <c r="C27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1111,7 +1121,7 @@
     </row>
     <row r="28" ht="14.25">
       <c r="C28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1119,23 +1129,29 @@
     </row>
     <row r="29" ht="14.25">
       <c r="C29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" ht="14.25">
       <c r="C30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
+      <c r="E30" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" ht="14.25">
       <c r="C31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1143,56 +1159,56 @@
     </row>
     <row r="32" ht="14.25">
       <c r="C32" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="C33" s="3" t="s">
-        <v>50</v>
+      <c r="C33" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="3"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="C37" s="3"/>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" ht="14.25">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1200,10 +1216,10 @@
     </row>
     <row r="39" ht="14.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1211,24 +1227,24 @@
     </row>
     <row r="40" ht="14.25">
       <c r="B40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="7" t="s">
         <v>57</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" ht="14.25">
       <c r="B42" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -1236,10 +1252,10 @@
     </row>
     <row r="43" ht="14.25">
       <c r="B43" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -1249,17 +1265,17 @@
     <row r="45" ht="14.25"/>
     <row r="46" ht="14.25">
       <c r="C46" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" ht="14.25">
       <c r="C47" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" ht="14.25">
       <c r="C48" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1270,6 +1286,9 @@
     <hyperlink r:id="rId4" ref="E9"/>
     <hyperlink r:id="rId5" ref="E10"/>
     <hyperlink r:id="rId6" ref="E24"/>
+    <hyperlink r:id="rId7" ref="E26"/>
+    <hyperlink r:id="rId8" ref="E29"/>
+    <hyperlink r:id="rId9" ref="E30"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>